<commit_message>
Updated CIV pretas forms
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Ivory Coast/civ_pretas_enrollement.xlsx
+++ b/LF/PreTAS/Ivory Coast/civ_pretas_enrollement.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\PreTAS\Ivory Coast\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbandubad\Repositories\dsa-forms\LF\PreTAS\Ivory Coast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20170957-6B44-4AE8-B8B5-0C4DA7CF954C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="25785" windowHeight="13980" tabRatio="548" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="134">
   <si>
     <t>type</t>
   </si>
@@ -131,9 +130,6 @@
     <t>select_one OuiNonSaitPas</t>
   </si>
   <si>
-    <t>select_one migration_list</t>
-  </si>
-  <si>
     <t>Hydrocèle</t>
   </si>
   <si>
@@ -284,9 +280,6 @@
     <t>${sexe}='M'</t>
   </si>
   <si>
-    <t>bf_pretas_lf_enrollement</t>
-  </si>
-  <si>
     <t>regex(., '^[0-9]{3}-[0-9]{4}$')</t>
   </si>
   <si>
@@ -350,9 +343,6 @@
     <t>Ghana</t>
   </si>
   <si>
-    <t>Aucun</t>
-  </si>
-  <si>
     <t>Autre région de la Côte d'Ivoire</t>
   </si>
   <si>
@@ -374,9 +364,6 @@
     <t>Veuillez précisez l'origine de la migration</t>
   </si>
   <si>
-    <t>Autre</t>
-  </si>
-  <si>
     <t xml:space="preserve"> migration_list</t>
   </si>
   <si>
@@ -389,9 +376,6 @@
     <t>Combien de fois avez reçu IVM+ALB au cours des cinq dernière années</t>
   </si>
   <si>
-    <t>2. Côte d'Ivoire - Pré TAS FL Formulaire Enrôlement</t>
-  </si>
-  <si>
     <t>ue</t>
   </si>
   <si>
@@ -425,16 +409,37 @@
     <t>Entrer le code du Site sentinnelle/Control Ponctuel</t>
   </si>
   <si>
-    <t>${migration_origine}='Autre'</t>
-  </si>
-  <si>
     <t>${migration}='Non'</t>
+  </si>
+  <si>
+    <t>Autre pays</t>
+  </si>
+  <si>
+    <t>Burkina.Faso</t>
+  </si>
+  <si>
+    <t>Autres.pays</t>
+  </si>
+  <si>
+    <t>Autre.region.de.la.cote.d.ivoire</t>
+  </si>
+  <si>
+    <t>selected(${migration_origine}, 'Autre.region.de.la.cote.d.ivoire')</t>
+  </si>
+  <si>
+    <t>select_multiple migration_list</t>
+  </si>
+  <si>
+    <t>bf_pretas_lf_enrollement_v2</t>
+  </si>
+  <si>
+    <t>2. Côte d'Ivoire - Pré TAS FL Formulaire Enrôlement V2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -685,7 +690,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -969,28 +974,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.87890625" customWidth="1"/>
-    <col min="5" max="5" width="14.5859375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.87890625" customWidth="1"/>
-    <col min="9" max="9" width="33.703125" customWidth="1"/>
-    <col min="11" max="11" width="28.52734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.7109375" customWidth="1"/>
+    <col min="11" max="11" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -998,10 +1003,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -1010,7 +1015,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
@@ -1022,90 +1027,90 @@
         <v>6</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
       <c r="J2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="J3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A4" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>125</v>
-      </c>
       <c r="C4" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C5" t="s">
+        <v>112</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>121</v>
-      </c>
       <c r="J5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="11"/>
       <c r="H6" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="11" t="s">
@@ -1115,22 +1120,22 @@
       <c r="L6" s="11"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="11"/>
       <c r="H7" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="11" t="s">
@@ -1140,115 +1145,115 @@
       <c r="L7" s="11"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
         <v>51</v>
       </c>
-      <c r="B8" t="s">
-        <v>52</v>
-      </c>
       <c r="C8" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
       <c r="H9" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" t="s">
         <v>73</v>
       </c>
-      <c r="J9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A10" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="J10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="C10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" t="s">
-        <v>86</v>
-      </c>
-      <c r="H10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A11" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" t="s">
-        <v>85</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>91</v>
-      </c>
       <c r="G11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
@@ -1257,12 +1262,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
@@ -1271,12 +1276,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
@@ -1285,148 +1290,148 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>113</v>
+      </c>
+      <c r="H17" t="s">
+        <v>90</v>
+      </c>
+      <c r="J17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
         <v>42</v>
       </c>
-      <c r="C17" t="s">
-        <v>117</v>
-      </c>
-      <c r="H17" t="s">
-        <v>92</v>
-      </c>
-      <c r="J17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A18" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" t="s">
-        <v>43</v>
-      </c>
       <c r="C18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" t="s">
+        <v>107</v>
+      </c>
+      <c r="H19" t="s">
+        <v>125</v>
+      </c>
+      <c r="J19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" t="s">
         <v>109</v>
-      </c>
-      <c r="J18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A19" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>107</v>
-      </c>
-      <c r="C19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D19" t="s">
-        <v>110</v>
-      </c>
-      <c r="H19" t="s">
-        <v>131</v>
-      </c>
-      <c r="J19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A20" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" t="s">
-        <v>108</v>
-      </c>
-      <c r="C20" t="s">
-        <v>112</v>
       </c>
       <c r="H20" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="17.350000000000001" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H21" s="10"/>
       <c r="J21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.5">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
     </row>
   </sheetData>
@@ -1436,21 +1441,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.29296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1458,10 +1463,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1469,10 +1474,10 @@
         <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1480,133 +1485,133 @@
         <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
         <v>52</v>
       </c>
-      <c r="B11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A12" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>10</v>
@@ -1615,9 +1620,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16">
         <v>11</v>
@@ -1626,9 +1631,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17">
         <v>12</v>
@@ -1637,9 +1642,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18">
         <v>13</v>
@@ -1648,9 +1653,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19">
         <v>14</v>
@@ -1659,9 +1664,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20">
         <v>15</v>
@@ -1670,9 +1675,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21">
         <v>16</v>
@@ -1681,9 +1686,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22">
         <v>17</v>
@@ -1692,9 +1697,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23">
         <v>18</v>
@@ -1703,9 +1708,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24">
         <v>19</v>
@@ -1714,81 +1719,81 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" t="s">
         <v>100</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A27" t="s">
-        <v>114</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" t="s">
         <v>101</v>
       </c>
-      <c r="C27" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A28" t="s">
-        <v>114</v>
-      </c>
-      <c r="B28" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" t="s">
         <v>102</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A29" t="s">
-        <v>114</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" t="s">
         <v>103</v>
-      </c>
-      <c r="C29" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A30" t="s">
-        <v>114</v>
-      </c>
-      <c r="B30" t="s">
-        <v>104</v>
-      </c>
-      <c r="C30" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A31" t="s">
-        <v>114</v>
-      </c>
-      <c r="B31" t="s">
-        <v>113</v>
-      </c>
-      <c r="C31" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1797,21 +1802,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.41015625" customWidth="1"/>
-    <col min="3" max="3" width="11.1171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -1819,24 +1824,24 @@
         <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="C2">
         <v>20200310</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some improvements on ivory coast fors.
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Ivory Coast/civ_pretas_enrollement.xlsx
+++ b/LF/PreTAS/Ivory Coast/civ_pretas_enrollement.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="25785" windowHeight="13980" tabRatio="548" activeTab="1"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="25785" windowHeight="13980" tabRatio="548"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="130">
   <si>
     <t>type</t>
   </si>
@@ -235,12 +236,6 @@
     <t>ouinon</t>
   </si>
   <si>
-    <t>${optionscanner}='scanner'</t>
-  </si>
-  <si>
-    <t>${optionscanner}='manuel'</t>
-  </si>
-  <si>
     <t>Lymphodeme</t>
   </si>
   <si>
@@ -262,24 +257,6 @@
     <t>hint::French</t>
   </si>
   <si>
-    <t>${sexe}='M'</t>
-  </si>
-  <si>
-    <t>regex(., '^[0-9]{3}-[0-9]{4}$')</t>
-  </si>
-  <si>
-    <t>Exemple "100-0001"</t>
-  </si>
-  <si>
-    <t>Le format est incorrect. Il doit être du type 123-1234</t>
-  </si>
-  <si>
-    <t>code_genere</t>
-  </si>
-  <si>
-    <t>${ivm_alb}='Oui'</t>
-  </si>
-  <si>
     <t>Ne.sais.pas</t>
   </si>
   <si>
@@ -361,9 +338,6 @@
     <t>code_site2</t>
   </si>
   <si>
-    <t>${migration}='Non'</t>
-  </si>
-  <si>
     <t>Autre pays</t>
   </si>
   <si>
@@ -376,15 +350,9 @@
     <t>Autre.region.de.la.cote.d.ivoire</t>
   </si>
   <si>
-    <t>selected(${migration_origine}, 'Autre.region.de.la.cote.d.ivoire')</t>
-  </si>
-  <si>
     <t>select_multiple migration_list</t>
   </si>
   <si>
-    <t>Veuillez sauvegarder ce code généré. Il sera utilisé pour identifier ce participant à cette enquête.</t>
-  </si>
-  <si>
     <t>read_only</t>
   </si>
   <si>
@@ -397,17 +365,71 @@
     <t>Site sentinelle/control ponctuel</t>
   </si>
   <si>
-    <t>bf_pretas_lf_enrollement_v3</t>
-  </si>
-  <si>
-    <t>2. Côte d'Ivoire - Pré TAS FL Formulaire Enrôlement V3</t>
+    <t>2. Côte d'Ivoire - Pré TAS FL Formulaire Enrôlement V4</t>
+  </si>
+  <si>
+    <t>bf_pretas_lf_enrollement_v4</t>
+  </si>
+  <si>
+    <t>consentement</t>
+  </si>
+  <si>
+    <t>Le répondant a-t-il donné son consentement?</t>
+  </si>
+  <si>
+    <t>Non mettra fin à l'enquête</t>
+  </si>
+  <si>
+    <t>code_id</t>
+  </si>
+  <si>
+    <t>Exemple "145001"</t>
+  </si>
+  <si>
+    <t>regex(., '^[0-9]{6}$')</t>
+  </si>
+  <si>
+    <t>Le format est incorrect. Cela doit être un nombre à six chiffre.</t>
+  </si>
+  <si>
+    <t>${consentement} = 'Oui'</t>
+  </si>
+  <si>
+    <t>${optionscanner}='scanner' and ${consentement} = 'Oui'</t>
+  </si>
+  <si>
+    <t>${optionscanner}='manuel' and ${consentement} = 'Oui'</t>
+  </si>
+  <si>
+    <t>${ivm_alb}='Oui' and ${consentement} = 'Oui'</t>
+  </si>
+  <si>
+    <t>${migration}='Non' and ${consentement} = 'Oui'</t>
+  </si>
+  <si>
+    <t>selected(${migration_origine}, 'Autre.region.de.la.cote.d.ivoire') and ${consentement} = 'Oui'</t>
+  </si>
+  <si>
+    <t>${sexe}='M' and ${consentement} = 'Oui'</t>
+  </si>
+  <si>
+    <t>Code d’identification du répondant</t>
+  </si>
+  <si>
+    <t>Répéter le code d’identification du répondant</t>
+  </si>
+  <si>
+    <t>code_id2</t>
+  </si>
+  <si>
+    <t>. = ${code_id}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,11 +480,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica"/>
     </font>
     <font>
       <sz val="12"/>
@@ -567,7 +584,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -586,13 +603,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -949,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,7 +996,7 @@
         <v>44</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -1001,16 +1017,16 @@
         <v>6</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1032,10 +1048,10 @@
         <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="J3" t="s">
         <v>10</v>
@@ -1046,10 +1062,10 @@
         <v>51</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="J4" t="s">
         <v>10</v>
@@ -1060,13 +1076,13 @@
         <v>51</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="J5" t="s">
         <v>10</v>
@@ -1077,24 +1093,24 @@
         <v>51</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="11"/>
+        <v>107</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="10"/>
       <c r="H6" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+        <v>97</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1102,52 +1118,61 @@
         <v>51</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
+        <v>97</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" t="s">
-        <v>10</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" t="s">
-        <v>67</v>
+        <v>46</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="J9" t="s">
         <v>10</v>
@@ -1155,30 +1180,18 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
-      </c>
-      <c r="D10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="J10" t="s">
-        <v>10</v>
-      </c>
-      <c r="N10" s="14" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1187,44 +1200,73 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>115</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" t="s">
-        <v>83</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>84</v>
+        <v>126</v>
+      </c>
+      <c r="D11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" t="s">
+        <v>121</v>
       </c>
       <c r="J11" t="s">
         <v>10</v>
       </c>
+      <c r="N11" s="13"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>127</v>
+      </c>
+      <c r="D12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" t="s">
+        <v>118</v>
+      </c>
+      <c r="H12" t="s">
+        <v>121</v>
       </c>
       <c r="J12" t="s">
         <v>10</v>
       </c>
+      <c r="N12" s="13"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" t="s">
+        <v>119</v>
       </c>
       <c r="J13" t="s">
         <v>10</v>
@@ -1232,16 +1274,16 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>17</v>
       </c>
       <c r="H14" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="J14" t="s">
         <v>10</v>
@@ -1249,16 +1291,16 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="H15" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="J15" t="s">
         <v>10</v>
@@ -1266,33 +1308,33 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>93</v>
+        <v>69</v>
+      </c>
+      <c r="H16" t="s">
+        <v>122</v>
       </c>
       <c r="J16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>115</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H17" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="J17" t="s">
         <v>10</v>
@@ -1300,79 +1342,118 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="H18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="J18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" s="10"/>
+        <v>83</v>
+      </c>
+      <c r="C19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" t="s">
+        <v>86</v>
+      </c>
+      <c r="H19" t="s">
+        <v>123</v>
+      </c>
       <c r="J19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>59</v>
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>88</v>
       </c>
       <c r="H20" t="s">
-        <v>76</v>
-      </c>
-      <c r="J20" t="s">
-        <v>10</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" t="s">
-        <v>41</v>
+        <v>61</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" t="s">
+        <v>119</v>
+      </c>
+      <c r="J21" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>98</v>
+      <c r="A22" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>60</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H22" t="s">
+        <v>125</v>
+      </c>
+      <c r="J22" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1384,8 +1465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1455,7 +1536,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
         <v>26</v>
@@ -1477,7 +1558,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>29</v>
@@ -1639,79 +1720,79 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C26" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B28" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1724,7 +1805,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,21 +1826,21 @@
         <v>65</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C2">
-        <v>20200310</v>
+        <v>20200320</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated ivory coast froms.
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Ivory Coast/civ_pretas_enrollement.xlsx
+++ b/LF/PreTAS/Ivory Coast/civ_pretas_enrollement.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbandubad\Repositories\dsa-forms\LF\PreTAS\Ivory Coast\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\PreTAS\Ivory Coast\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF14B1F1-BC9D-41BD-BC42-235A3C066789}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="25785" windowHeight="13980" tabRatio="548"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="548" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,6 @@
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="115">
   <si>
     <t>type</t>
   </si>
@@ -77,12 +77,6 @@
     <t>integer</t>
   </si>
   <si>
-    <t>barcode</t>
-  </si>
-  <si>
-    <t>Code barre</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
@@ -134,9 +128,6 @@
     <t>sexe</t>
   </si>
   <si>
-    <t>code_barre</t>
-  </si>
-  <si>
     <t>ivm_alb</t>
   </si>
   <si>
@@ -170,24 +161,6 @@
     <t>label::French</t>
   </si>
   <si>
-    <t>select_one optionscanner</t>
-  </si>
-  <si>
-    <t>optionscanner</t>
-  </si>
-  <si>
-    <t>manuel</t>
-  </si>
-  <si>
-    <t>scanner</t>
-  </si>
-  <si>
-    <t>Scanner</t>
-  </si>
-  <si>
-    <t>Manuel</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -227,9 +200,6 @@
     <t>commentaires</t>
   </si>
   <si>
-    <t>Souhaitez-vous scanner ou saisir manuellement le code-barres?</t>
-  </si>
-  <si>
     <t>version</t>
   </si>
   <si>
@@ -365,12 +335,6 @@
     <t>Site sentinelle/control ponctuel</t>
   </si>
   <si>
-    <t>2. Côte d'Ivoire - Pré TAS FL Formulaire Enrôlement V4</t>
-  </si>
-  <si>
-    <t>bf_pretas_lf_enrollement_v4</t>
-  </si>
-  <si>
     <t>consentement</t>
   </si>
   <si>
@@ -383,24 +347,12 @@
     <t>code_id</t>
   </si>
   <si>
-    <t>Exemple "145001"</t>
-  </si>
-  <si>
-    <t>regex(., '^[0-9]{6}$')</t>
-  </si>
-  <si>
     <t>Le format est incorrect. Cela doit être un nombre à six chiffre.</t>
   </si>
   <si>
     <t>${consentement} = 'Oui'</t>
   </si>
   <si>
-    <t>${optionscanner}='scanner' and ${consentement} = 'Oui'</t>
-  </si>
-  <si>
-    <t>${optionscanner}='manuel' and ${consentement} = 'Oui'</t>
-  </si>
-  <si>
     <t>${ivm_alb}='Oui' and ${consentement} = 'Oui'</t>
   </si>
   <si>
@@ -416,19 +368,22 @@
     <t>Code d’identification du répondant</t>
   </si>
   <si>
-    <t>Répéter le code d’identification du répondant</t>
-  </si>
-  <si>
-    <t>code_id2</t>
-  </si>
-  <si>
-    <t>. = ${code_id}</t>
+    <t>Exemple "145-123456"</t>
+  </si>
+  <si>
+    <t>2. Côte d'Ivoire - Pré TAS FL Formulaire Enrôlement V5</t>
+  </si>
+  <si>
+    <t>concat(${code_site}, ${code_site2}, '-', substr(random(),3,9))</t>
+  </si>
+  <si>
+    <t>ci_pretas_lf_enrollement_v5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -495,7 +450,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -505,12 +460,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,7 +533,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -602,7 +551,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -680,7 +628,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -964,28 +912,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.87890625" customWidth="1"/>
+    <col min="5" max="5" width="14.5859375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.7109375" customWidth="1"/>
-    <col min="11" max="11" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.703125" customWidth="1"/>
+    <col min="11" max="11" width="28.5859375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -993,10 +941,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -1005,7 +953,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
@@ -1017,443 +965,387 @@
         <v>6</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9" t="s">
+        <v>113</v>
+      </c>
+      <c r="J9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" t="s">
+        <v>105</v>
+      </c>
+      <c r="J10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
+        <v>105</v>
+      </c>
+      <c r="J11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="J3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="J4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="J5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="J13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" t="s">
+        <v>106</v>
+      </c>
+      <c r="J14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A15" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="J9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" t="s">
-        <v>120</v>
-      </c>
-      <c r="J10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" t="s">
-        <v>126</v>
-      </c>
-      <c r="D11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="G11" t="s">
-        <v>118</v>
-      </c>
-      <c r="H11" t="s">
-        <v>121</v>
-      </c>
-      <c r="J11" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11" s="13"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>128</v>
-      </c>
-      <c r="C12" t="s">
-        <v>127</v>
-      </c>
-      <c r="D12" t="s">
-        <v>116</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="G12" t="s">
-        <v>118</v>
-      </c>
-      <c r="H12" t="s">
-        <v>121</v>
-      </c>
-      <c r="J12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N12" s="13"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="H13" t="s">
-        <v>119</v>
-      </c>
-      <c r="J13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" t="s">
-        <v>119</v>
-      </c>
-      <c r="J14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="H15" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="J15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A16" s="5" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
       <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H16" t="s">
+        <v>107</v>
+      </c>
+      <c r="J16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" t="s">
+        <v>105</v>
+      </c>
+      <c r="J18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" t="s">
+        <v>109</v>
+      </c>
+      <c r="J19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C16" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" t="s">
-        <v>122</v>
-      </c>
-      <c r="J16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H17" t="s">
-        <v>122</v>
-      </c>
-      <c r="J17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" t="s">
-        <v>85</v>
-      </c>
-      <c r="H18" t="s">
-        <v>119</v>
-      </c>
-      <c r="J18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B19" t="s">
-        <v>83</v>
-      </c>
-      <c r="C19" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" t="s">
-        <v>86</v>
-      </c>
-      <c r="H19" t="s">
-        <v>123</v>
-      </c>
-      <c r="J19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" t="s">
-        <v>88</v>
-      </c>
-      <c r="H20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="B22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="H22" t="s">
-        <v>125</v>
-      </c>
-      <c r="J22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>90</v>
-      </c>
-      <c r="B24" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1462,21 +1354,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A9" sqref="A9:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.29296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1484,315 +1376,293 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C7" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C8" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A9" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="B9" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10" s="7" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B14">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B15">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B16">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C16">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B17">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C17">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B18">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C18">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B19">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C19">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B20">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C20">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21">
-        <v>18</v>
-      </c>
-      <c r="C21">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22">
-        <v>19</v>
-      </c>
-      <c r="C22">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
         <v>79</v>
       </c>
-      <c r="C25" t="s">
+      <c r="B26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>89</v>
-      </c>
-      <c r="B26" t="s">
-        <v>102</v>
-      </c>
-      <c r="C26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>89</v>
-      </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>89</v>
-      </c>
-      <c r="B28" t="s">
-        <v>103</v>
-      </c>
-      <c r="C28" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>89</v>
-      </c>
-      <c r="B29" t="s">
-        <v>104</v>
-      </c>
-      <c r="C29" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1801,21 +1671,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="56" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.41015625" customWidth="1"/>
+    <col min="3" max="3" width="11.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -1823,27 +1693,28 @@
         <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C2">
-        <v>20200320</v>
+        <v>20200817</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
some updates on civ pretas form.
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Ivory Coast/civ_pretas_enrollement.xlsx
+++ b/LF/PreTAS/Ivory Coast/civ_pretas_enrollement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\PreTAS\Ivory Coast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF14B1F1-BC9D-41BD-BC42-235A3C066789}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8925E8C4-2418-486E-B6DA-A8B8085B5A10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="548" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11070" tabRatio="548" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -371,13 +371,13 @@
     <t>Exemple "145-123456"</t>
   </si>
   <si>
-    <t>2. Côte d'Ivoire - Pré TAS FL Formulaire Enrôlement V5</t>
-  </si>
-  <si>
     <t>concat(${code_site}, ${code_site2}, '-', substr(random(),3,9))</t>
   </si>
   <si>
-    <t>ci_pretas_lf_enrollement_v5</t>
+    <t>2. Côte d'Ivoire - Pré TAS FL Formulaire Enrôlement V6</t>
+  </si>
+  <si>
+    <t>ci_pretas_lf_enrollement_v6</t>
   </si>
 </sst>
 </file>
@@ -919,21 +919,21 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.87890625" customWidth="1"/>
-    <col min="5" max="5" width="14.5859375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.703125" customWidth="1"/>
-    <col min="11" max="11" width="28.5859375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.7109375" customWidth="1"/>
+    <col min="11" max="11" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -977,7 +977,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>42</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>42</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>42</v>
       </c>
@@ -1061,7 +1061,7 @@
       <c r="L6" s="9"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:14" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>42</v>
       </c>
@@ -1086,7 +1086,7 @@
       <c r="L7" s="9"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:14" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>46</v>
       </c>
@@ -1111,7 +1111,7 @@
       <c r="L8" s="9"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>42</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>105</v>
       </c>
       <c r="I9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J9" t="s">
         <v>10</v>
@@ -1141,7 +1141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>25</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>46</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>95</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>42</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>46</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>46</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>9</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>35</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
     </row>
   </sheetData>
@@ -1361,14 +1361,14 @@
       <selection activeCell="A9" sqref="A9:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.29296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.1171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>56</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>56</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -1675,17 +1675,17 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.41015625" customWidth="1"/>
-    <col min="3" max="3" width="11.1171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -1699,15 +1699,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
         <v>114</v>
       </c>
       <c r="C2">
-        <v>20200817</v>
+        <v>20200819</v>
       </c>
       <c r="D2" t="s">
         <v>61</v>

</xml_diff>